<commit_message>
difficulty level image renders on cards
</commit_message>
<xml_diff>
--- a/Project Management/IC-Agile-User-Story-Template-8561.xlsx
+++ b/Project Management/IC-Agile-User-Story-Template-8561.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zacharymargolies/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zacharymargolies/Desktop/coding/coding-question-trivia/Project Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0385A5AE-DFC1-4A42-B22E-3237775B21BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB424B2-AC5B-2240-9D72-E1C7C4B7B5BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-660" yWindow="-20400" windowWidth="30280" windowHeight="19240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile User Story" sheetId="1" r:id="rId1"/>
@@ -696,9 +696,9 @@
   </sheetPr>
   <dimension ref="B1:N65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -773,7 +773,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -908,7 +908,7 @@
         <v>19</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -989,7 +989,7 @@
         <v>24</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1070,7 +1070,7 @@
         <v>30</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1097,7 +1097,7 @@
         <v>32</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>

</xml_diff>